<commit_message>
Mise à jour polygones ASTAR
</commit_message>
<xml_diff>
--- a/2_Strategie/PolygonesASTAR.xlsx
+++ b/2_Strategie/PolygonesASTAR.xlsx
@@ -29,18 +29,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Courier"/>
     </font>
     <font>
       <sz val="12"/>
@@ -69,16 +64,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,10 +139,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.328054853193037E-2"/>
-          <c:y val="7.1375266742601404E-2"/>
+          <c:x val="2.9118065373576196E-2"/>
+          <c:y val="8.9358370019413297E-2"/>
           <c:w val="0.86865958453296255"/>
-          <c:h val="0.88398244298417139"/>
+          <c:h val="0.84981443380717248"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1266,12 +1257,400 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="42"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="43"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="44"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="50"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="51"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="52"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="58"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="59"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="60"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="61"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="62"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="63"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="64"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7030A0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$A$1:$A$42</c:f>
+              <c:f>Feuil1!$A$1:$A$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -1396,17 +1775,86 @@
                   <c:v>354</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1346</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1346</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1275</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$B$42</c:f>
+              <c:f>Feuil1!$B$1:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="65"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1531,7 +1979,76 @@
                   <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2446</c:v>
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2454</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2524</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2596</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2104</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2104</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2596</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2454</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2524</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1546,11 +2063,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-609418448"/>
-        <c:axId val="-609417904"/>
+        <c:axId val="-2145191504"/>
+        <c:axId val="-2145199120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-609418448"/>
+        <c:axId val="-2145191504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -1608,12 +2125,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-609417904"/>
+        <c:crossAx val="-2145199120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-609417904"/>
+        <c:axId val="-2145199120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3000"/>
@@ -1671,7 +2188,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-609418448"/>
+        <c:crossAx val="-2145191504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2574,10 +3091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,7 +3106,7 @@
       <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -2598,7 +3115,7 @@
       <c r="B2" s="1">
         <v>496</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2607,7 +3124,7 @@
       <c r="B3" s="1">
         <v>439</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -2616,7 +3133,7 @@
       <c r="B4" s="1">
         <v>248</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2625,7 +3142,7 @@
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -2634,7 +3151,7 @@
       <c r="B6" s="1">
         <v>3000</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2643,7 +3160,7 @@
       <c r="B7" s="1">
         <v>3000</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -2652,7 +3169,7 @@
       <c r="B8" s="1">
         <v>2752</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -2661,7 +3178,7 @@
       <c r="B9" s="1">
         <v>2560</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2670,7 +3187,7 @@
       <c r="B10" s="1">
         <v>2504</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2679,7 +3196,7 @@
       <c r="B11" s="1">
         <v>2346</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2688,7 +3205,7 @@
       <c r="B12" s="1">
         <v>2275</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2697,7 +3214,7 @@
       <c r="B13" s="1">
         <v>2100</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2706,7 +3223,7 @@
       <c r="B14" s="1">
         <v>1500</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2715,7 +3232,7 @@
       <c r="B15" s="1">
         <v>900</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2724,7 +3241,7 @@
       <c r="B16" s="1">
         <v>724</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2733,7 +3250,7 @@
       <c r="B17" s="1">
         <v>654</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2742,7 +3259,7 @@
       <c r="B18" s="1">
         <v>718</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -2751,7 +3268,7 @@
       <c r="B19" s="1">
         <v>901</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -2760,7 +3277,7 @@
       <c r="B20" s="1">
         <v>1176</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -2769,9 +3286,9 @@
       <c r="B21" s="1">
         <v>1500</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1536</v>
       </c>
@@ -2786,7 +3303,7 @@
       <c r="B23" s="1">
         <v>2098</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -2795,7 +3312,7 @@
       <c r="B24" s="1">
         <v>2281</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -2804,7 +3321,7 @@
       <c r="B25" s="1">
         <v>554</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -2813,7 +3330,7 @@
       <c r="B26" s="1">
         <v>554</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -2822,7 +3339,7 @@
       <c r="B27" s="1">
         <v>624</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -2831,7 +3348,7 @@
       <c r="B28" s="1">
         <v>800</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -2840,9 +3357,9 @@
       <c r="B29" s="1">
         <v>1500</v>
       </c>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>446</v>
       </c>
@@ -2857,7 +3374,7 @@
       <c r="B31" s="1">
         <v>2375</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -2866,7 +3383,7 @@
       <c r="B32" s="1">
         <v>2446</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -2875,7 +3392,7 @@
       <c r="B33" s="1">
         <v>2446</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -2884,7 +3401,7 @@
       <c r="B34" s="1">
         <v>3000</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -2893,7 +3410,7 @@
       <c r="B35" s="1">
         <v>2700</v>
       </c>
-      <c r="C35" s="3"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -2902,9 +3419,9 @@
       <c r="B36" s="1">
         <v>2524</v>
       </c>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1100</v>
       </c>
@@ -2912,7 +3429,7 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>600</v>
       </c>
@@ -2920,7 +3437,7 @@
         <v>2454</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>424</v>
       </c>
@@ -2928,7 +3445,7 @@
         <v>2524</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>354</v>
       </c>
@@ -2936,7 +3453,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>354</v>
       </c>
@@ -2944,124 +3461,196 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
+        <v>1146</v>
+      </c>
+      <c r="B42" s="1">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1146</v>
+      </c>
+      <c r="B43" s="1">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>654</v>
+      </c>
+      <c r="B44" s="1">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>654</v>
+      </c>
+      <c r="B45" s="1">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>424</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>354</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>354</v>
+      </c>
+      <c r="B49" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>1146</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>1146</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>654</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>654</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>600</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>424</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2524</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>354</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>354</v>
+      </c>
+      <c r="B57" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>1346</v>
+      </c>
+      <c r="B58" s="1">
         <v>0</v>
       </c>
-      <c r="B42" s="1">
-        <v>2446</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>1536</v>
-      </c>
-      <c r="B43" s="1">
-        <v>1176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>1640</v>
-      </c>
-      <c r="B44" s="1">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>1409</v>
-      </c>
-      <c r="B45" s="1">
-        <v>1278</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>951</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1278</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>720</v>
-      </c>
-      <c r="B47" s="1">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>951</v>
-      </c>
-      <c r="B48" s="1">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>1409</v>
-      </c>
-      <c r="B49" s="1">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>900</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>669</v>
-      </c>
-      <c r="B51" s="1">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>211</v>
-      </c>
-      <c r="B52" s="1">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>-20</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>211</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>669</v>
-      </c>
-      <c r="B55" s="2">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>500</v>
-      </c>
-      <c r="B56" s="1">
-        <v>2300</v>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>1346</v>
+      </c>
+      <c r="B59" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>1275</v>
+      </c>
+      <c r="B60" s="1">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>1100</v>
+      </c>
+      <c r="B61" s="1">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>600</v>
+      </c>
+      <c r="B62" s="1">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>424</v>
+      </c>
+      <c r="B63" s="1">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>354</v>
+      </c>
+      <c r="B64" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>354</v>
+      </c>
+      <c r="B65" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>